<commit_message>
Help menu, bug fixes
</commit_message>
<xml_diff>
--- a/data/reference_data.xlsx
+++ b/data/reference_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Code\WebstormProjects\TB_QBO_Converter\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49DD60B9-8648-47E6-A0AA-03DFDCE96106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA75C98C-CD0D-4C46-B21D-4F619EE4A394}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51480" yWindow="5295" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Categories" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="DetailTypes" sheetId="3" r:id="rId3"/>
     <sheet name="GIFI" sheetId="5" r:id="rId4"/>
     <sheet name="Keywords" sheetId="6" r:id="rId5"/>
+    <sheet name="CategoryIndicators" sheetId="7" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4150" uniqueCount="2254">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4063" uniqueCount="2263">
   <si>
     <t>Category</t>
   </si>
@@ -6799,6 +6800,33 @@
   </si>
   <si>
     <t>REVENUS D'INTÉRÊTS</t>
+  </si>
+  <si>
+    <t>IsDefault</t>
+  </si>
+  <si>
+    <t>IsFallback</t>
+  </si>
+  <si>
+    <t>Points</t>
+  </si>
+  <si>
+    <t>A/P</t>
+  </si>
+  <si>
+    <t>CHARGES</t>
+  </si>
+  <si>
+    <t>EXPENSE</t>
+  </si>
+  <si>
+    <t>DÉPENSE</t>
+  </si>
+  <si>
+    <t>DÉPENSES</t>
+  </si>
+  <si>
+    <t>FRAIS</t>
   </si>
 </sst>
 </file>
@@ -7642,10 +7670,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:E130"/>
+  <dimension ref="A1:F130"/>
   <sheetViews>
-    <sheetView topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="D108" sqref="D108"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="F71" sqref="F71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -7653,10 +7681,10 @@
     <col min="1" max="1" width="22.59765625" customWidth="1"/>
     <col min="2" max="2" width="20.59765625" customWidth="1"/>
     <col min="3" max="3" width="44.59765625" customWidth="1"/>
-    <col min="4" max="4" width="66.8984375" customWidth="1"/>
+    <col min="4" max="4" width="68.796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>1851</v>
       </c>
@@ -7669,8 +7697,14 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>2254</v>
+      </c>
+      <c r="F1" t="s">
+        <v>2255</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1716</v>
       </c>
@@ -7681,13 +7715,13 @@
         <v>34</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1716</v>
       </c>
@@ -7698,13 +7732,10 @@
         <v>41</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
         <v>1860</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1716</v>
       </c>
@@ -7715,13 +7746,10 @@
         <v>36</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>1716</v>
       </c>
@@ -7732,13 +7760,10 @@
         <v>42</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
         <v>1863</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>1716</v>
       </c>
@@ -7749,13 +7774,10 @@
         <v>43</v>
       </c>
       <c r="D6" t="s">
-        <v>17</v>
-      </c>
-      <c r="E6" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>1716</v>
       </c>
@@ -7766,13 +7788,10 @@
         <v>38</v>
       </c>
       <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>45</v>
       </c>
@@ -7785,11 +7804,11 @@
       <c r="D8" t="s">
         <v>1841</v>
       </c>
-      <c r="E8" t="s">
-        <v>1841</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E8" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>1852</v>
       </c>
@@ -7800,13 +7819,16 @@
         <v>64</v>
       </c>
       <c r="D9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E9" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E9" t="b">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>1852</v>
       </c>
@@ -7817,13 +7839,10 @@
         <v>70</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
-      </c>
-      <c r="E10" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>1852</v>
       </c>
@@ -7834,13 +7853,10 @@
         <v>52</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
-      </c>
-      <c r="E11" t="s">
         <v>1869</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>1852</v>
       </c>
@@ -7851,13 +7867,10 @@
         <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
-      </c>
-      <c r="E12" t="s">
         <v>1871</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>1852</v>
       </c>
@@ -7868,13 +7881,10 @@
         <v>72</v>
       </c>
       <c r="D13" t="s">
-        <v>20</v>
-      </c>
-      <c r="E13" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>1852</v>
       </c>
@@ -7885,13 +7895,10 @@
         <v>49</v>
       </c>
       <c r="D14" t="s">
-        <v>20</v>
-      </c>
-      <c r="E14" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>1852</v>
       </c>
@@ -7902,13 +7909,10 @@
         <v>54</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
-      </c>
-      <c r="E15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>1852</v>
       </c>
@@ -7919,9 +7923,6 @@
         <v>48</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
-      </c>
-      <c r="E16" t="s">
         <v>1876</v>
       </c>
     </row>
@@ -7936,9 +7937,6 @@
         <v>1878</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
-      </c>
-      <c r="E17" t="s">
         <v>62</v>
       </c>
     </row>
@@ -7953,9 +7951,6 @@
         <v>57</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
-      </c>
-      <c r="E18" t="s">
         <v>58</v>
       </c>
     </row>
@@ -7970,9 +7965,6 @@
         <v>60</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
-      </c>
-      <c r="E19" t="s">
         <v>1881</v>
       </c>
     </row>
@@ -7987,9 +7979,6 @@
         <v>68</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E20" t="s">
         <v>1883</v>
       </c>
     </row>
@@ -8004,9 +7993,6 @@
         <v>90</v>
       </c>
       <c r="D21" t="s">
-        <v>1842</v>
-      </c>
-      <c r="E21" t="s">
         <v>91</v>
       </c>
     </row>
@@ -8021,10 +8007,10 @@
         <v>417</v>
       </c>
       <c r="D22" t="s">
-        <v>1842</v>
-      </c>
-      <c r="E22" t="s">
         <v>1886</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
@@ -8038,9 +8024,6 @@
         <v>82</v>
       </c>
       <c r="D23" t="s">
-        <v>1842</v>
-      </c>
-      <c r="E23" t="s">
         <v>83</v>
       </c>
     </row>
@@ -8055,9 +8038,6 @@
         <v>92</v>
       </c>
       <c r="D24" t="s">
-        <v>1842</v>
-      </c>
-      <c r="E24" t="s">
         <v>93</v>
       </c>
     </row>
@@ -8072,9 +8052,6 @@
         <v>74</v>
       </c>
       <c r="D25" t="s">
-        <v>1842</v>
-      </c>
-      <c r="E25" t="s">
         <v>75</v>
       </c>
     </row>
@@ -8089,9 +8066,6 @@
         <v>1891</v>
       </c>
       <c r="D26" t="s">
-        <v>1842</v>
-      </c>
-      <c r="E26" t="s">
         <v>1892</v>
       </c>
     </row>
@@ -8106,9 +8080,6 @@
         <v>85</v>
       </c>
       <c r="D27" t="s">
-        <v>1842</v>
-      </c>
-      <c r="E27" t="s">
         <v>1894</v>
       </c>
     </row>
@@ -8123,9 +8094,6 @@
         <v>77</v>
       </c>
       <c r="D28" t="s">
-        <v>1842</v>
-      </c>
-      <c r="E28" t="s">
         <v>78</v>
       </c>
     </row>
@@ -8140,9 +8108,6 @@
         <v>87</v>
       </c>
       <c r="D29" t="s">
-        <v>1842</v>
-      </c>
-      <c r="E29" t="s">
         <v>88</v>
       </c>
     </row>
@@ -8157,9 +8122,6 @@
         <v>95</v>
       </c>
       <c r="D30" t="s">
-        <v>1843</v>
-      </c>
-      <c r="E30" t="s">
         <v>1898</v>
       </c>
     </row>
@@ -8174,10 +8136,10 @@
         <v>107</v>
       </c>
       <c r="D31" t="s">
-        <v>1843</v>
-      </c>
-      <c r="E31" t="s">
         <v>108</v>
+      </c>
+      <c r="E31" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.3">
@@ -8191,13 +8153,10 @@
         <v>110</v>
       </c>
       <c r="D32" t="s">
-        <v>1843</v>
-      </c>
-      <c r="E32" t="s">
         <v>1900</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>106</v>
       </c>
@@ -8208,13 +8167,10 @@
         <v>102</v>
       </c>
       <c r="D33" t="s">
-        <v>1843</v>
-      </c>
-      <c r="E33" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>106</v>
       </c>
@@ -8225,13 +8181,10 @@
         <v>111</v>
       </c>
       <c r="D34" t="s">
-        <v>1843</v>
-      </c>
-      <c r="E34" t="s">
         <v>1903</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>106</v>
       </c>
@@ -8242,13 +8195,10 @@
         <v>96</v>
       </c>
       <c r="D35" t="s">
-        <v>1843</v>
-      </c>
-      <c r="E35" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>106</v>
       </c>
@@ -8259,13 +8209,10 @@
         <v>113</v>
       </c>
       <c r="D36" t="s">
-        <v>1843</v>
-      </c>
-      <c r="E36" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>106</v>
       </c>
@@ -8276,13 +8223,10 @@
         <v>104</v>
       </c>
       <c r="D37" t="s">
-        <v>1843</v>
-      </c>
-      <c r="E37" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>106</v>
       </c>
@@ -8293,13 +8237,10 @@
         <v>116</v>
       </c>
       <c r="D38" t="s">
-        <v>1843</v>
-      </c>
-      <c r="E38" t="s">
         <v>1908</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>106</v>
       </c>
@@ -8310,13 +8251,10 @@
         <v>99</v>
       </c>
       <c r="D39" t="s">
-        <v>1843</v>
-      </c>
-      <c r="E39" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>106</v>
       </c>
@@ -8327,13 +8265,10 @@
         <v>1911</v>
       </c>
       <c r="D40" t="s">
-        <v>1843</v>
-      </c>
-      <c r="E40" t="s">
         <v>1912</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>106</v>
       </c>
@@ -8344,13 +8279,10 @@
         <v>118</v>
       </c>
       <c r="D41" t="s">
-        <v>1843</v>
-      </c>
-      <c r="E41" t="s">
         <v>1914</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>106</v>
       </c>
@@ -8361,13 +8293,10 @@
         <v>98</v>
       </c>
       <c r="D42" t="s">
-        <v>1843</v>
-      </c>
-      <c r="E42" t="s">
         <v>1916</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>119</v>
       </c>
@@ -8380,11 +8309,11 @@
       <c r="D43" t="s">
         <v>1844</v>
       </c>
-      <c r="E43" t="s">
-        <v>1844</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E43" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>121</v>
       </c>
@@ -8397,11 +8326,11 @@
       <c r="D44" t="s">
         <v>23</v>
       </c>
-      <c r="E44" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E44" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>1854</v>
       </c>
@@ -8412,13 +8341,16 @@
         <v>24</v>
       </c>
       <c r="D45" t="s">
-        <v>1845</v>
-      </c>
-      <c r="E45" t="s">
         <v>1918</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E45" t="b">
+        <v>1</v>
+      </c>
+      <c r="F45" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>1854</v>
       </c>
@@ -8429,13 +8361,10 @@
         <v>123</v>
       </c>
       <c r="D46" t="s">
-        <v>1845</v>
-      </c>
-      <c r="E46" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>1854</v>
       </c>
@@ -8446,13 +8375,10 @@
         <v>125</v>
       </c>
       <c r="D47" t="s">
-        <v>1845</v>
-      </c>
-      <c r="E47" t="s">
         <v>1921</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>1854</v>
       </c>
@@ -8463,9 +8389,6 @@
         <v>126</v>
       </c>
       <c r="D48" t="s">
-        <v>1845</v>
-      </c>
-      <c r="E48" t="s">
         <v>1923</v>
       </c>
     </row>
@@ -8480,9 +8403,6 @@
         <v>127</v>
       </c>
       <c r="D49" t="s">
-        <v>1845</v>
-      </c>
-      <c r="E49" t="s">
         <v>1925</v>
       </c>
     </row>
@@ -8497,9 +8417,6 @@
         <v>129</v>
       </c>
       <c r="D50" t="s">
-        <v>1845</v>
-      </c>
-      <c r="E50" t="s">
         <v>1927</v>
       </c>
     </row>
@@ -8514,9 +8431,6 @@
         <v>131</v>
       </c>
       <c r="D51" t="s">
-        <v>1845</v>
-      </c>
-      <c r="E51" t="s">
         <v>132</v>
       </c>
     </row>
@@ -8531,9 +8445,6 @@
         <v>134</v>
       </c>
       <c r="D52" t="s">
-        <v>1845</v>
-      </c>
-      <c r="E52" t="s">
         <v>1929</v>
       </c>
     </row>
@@ -8548,9 +8459,6 @@
         <v>135</v>
       </c>
       <c r="D53" t="s">
-        <v>1845</v>
-      </c>
-      <c r="E53" t="s">
         <v>1931</v>
       </c>
     </row>
@@ -8565,9 +8473,6 @@
         <v>137</v>
       </c>
       <c r="D54" t="s">
-        <v>1845</v>
-      </c>
-      <c r="E54" t="s">
         <v>1933</v>
       </c>
     </row>
@@ -8582,9 +8487,6 @@
         <v>138</v>
       </c>
       <c r="D55" t="s">
-        <v>1845</v>
-      </c>
-      <c r="E55" t="s">
         <v>1935</v>
       </c>
     </row>
@@ -8599,9 +8501,6 @@
         <v>139</v>
       </c>
       <c r="D56" t="s">
-        <v>1845</v>
-      </c>
-      <c r="E56" t="s">
         <v>1937</v>
       </c>
     </row>
@@ -8616,9 +8515,6 @@
         <v>141</v>
       </c>
       <c r="D57" t="s">
-        <v>1845</v>
-      </c>
-      <c r="E57" t="s">
         <v>142</v>
       </c>
     </row>
@@ -8633,9 +8529,6 @@
         <v>144</v>
       </c>
       <c r="D58" t="s">
-        <v>1845</v>
-      </c>
-      <c r="E58" t="s">
         <v>1940</v>
       </c>
     </row>
@@ -8650,9 +8543,6 @@
         <v>146</v>
       </c>
       <c r="D59" t="s">
-        <v>1845</v>
-      </c>
-      <c r="E59" t="s">
         <v>1942</v>
       </c>
     </row>
@@ -8667,10 +8557,10 @@
         <v>148</v>
       </c>
       <c r="D60" t="s">
-        <v>26</v>
-      </c>
-      <c r="E60" t="s">
         <v>149</v>
+      </c>
+      <c r="E60" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.3">
@@ -8684,9 +8574,6 @@
         <v>151</v>
       </c>
       <c r="D61" t="s">
-        <v>26</v>
-      </c>
-      <c r="E61" t="s">
         <v>1944</v>
       </c>
     </row>
@@ -8701,9 +8588,6 @@
         <v>153</v>
       </c>
       <c r="D62" t="s">
-        <v>26</v>
-      </c>
-      <c r="E62" t="s">
         <v>154</v>
       </c>
     </row>
@@ -8718,9 +8602,6 @@
         <v>156</v>
       </c>
       <c r="D63" t="s">
-        <v>26</v>
-      </c>
-      <c r="E63" t="s">
         <v>1947</v>
       </c>
     </row>
@@ -8735,13 +8616,10 @@
         <v>157</v>
       </c>
       <c r="D64" t="s">
-        <v>26</v>
-      </c>
-      <c r="E64" t="s">
         <v>1949</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>1855</v>
       </c>
@@ -8752,13 +8630,10 @@
         <v>158</v>
       </c>
       <c r="D65" t="s">
-        <v>26</v>
-      </c>
-      <c r="E65" t="s">
         <v>1951</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>1855</v>
       </c>
@@ -8769,13 +8644,10 @@
         <v>159</v>
       </c>
       <c r="D66" t="s">
-        <v>26</v>
-      </c>
-      <c r="E66" t="s">
         <v>1953</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>1855</v>
       </c>
@@ -8786,13 +8658,10 @@
         <v>161</v>
       </c>
       <c r="D67" t="s">
-        <v>26</v>
-      </c>
-      <c r="E67" t="s">
         <v>1955</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>1856</v>
       </c>
@@ -8803,13 +8672,10 @@
         <v>164</v>
       </c>
       <c r="D68" t="s">
-        <v>1846</v>
-      </c>
-      <c r="E68" t="s">
         <v>1957</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>1856</v>
       </c>
@@ -8820,13 +8686,10 @@
         <v>175</v>
       </c>
       <c r="D69" t="s">
-        <v>1846</v>
-      </c>
-      <c r="E69" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>1856</v>
       </c>
@@ -8837,13 +8700,16 @@
         <v>167</v>
       </c>
       <c r="D70" t="s">
-        <v>1846</v>
-      </c>
-      <c r="E70" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E70" t="b">
+        <v>1</v>
+      </c>
+      <c r="F70" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>1856</v>
       </c>
@@ -8854,13 +8720,10 @@
         <v>180</v>
       </c>
       <c r="D71" t="s">
-        <v>1846</v>
-      </c>
-      <c r="E71" t="s">
         <v>1960</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>1856</v>
       </c>
@@ -8871,13 +8734,10 @@
         <v>178</v>
       </c>
       <c r="D72" t="s">
-        <v>1846</v>
-      </c>
-      <c r="E72" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>1856</v>
       </c>
@@ -8888,13 +8748,10 @@
         <v>169</v>
       </c>
       <c r="D73" t="s">
-        <v>1846</v>
-      </c>
-      <c r="E73" t="s">
         <v>1962</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>1856</v>
       </c>
@@ -8905,13 +8762,10 @@
         <v>165</v>
       </c>
       <c r="D74" t="s">
-        <v>1846</v>
-      </c>
-      <c r="E74" t="s">
         <v>1964</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>1856</v>
       </c>
@@ -8922,13 +8776,10 @@
         <v>181</v>
       </c>
       <c r="D75" t="s">
-        <v>1846</v>
-      </c>
-      <c r="E75" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>1856</v>
       </c>
@@ -8939,13 +8790,10 @@
         <v>172</v>
       </c>
       <c r="D76" t="s">
-        <v>1846</v>
-      </c>
-      <c r="E76" t="s">
         <v>1967</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>1856</v>
       </c>
@@ -8956,13 +8804,10 @@
         <v>171</v>
       </c>
       <c r="D77" t="s">
-        <v>1846</v>
-      </c>
-      <c r="E77" t="s">
         <v>1969</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>1856</v>
       </c>
@@ -8973,13 +8818,10 @@
         <v>162</v>
       </c>
       <c r="D78" t="s">
-        <v>1846</v>
-      </c>
-      <c r="E78" t="s">
         <v>1971</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>1856</v>
       </c>
@@ -8990,13 +8832,10 @@
         <v>173</v>
       </c>
       <c r="D79" t="s">
-        <v>1846</v>
-      </c>
-      <c r="E79" t="s">
         <v>1973</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>186</v>
       </c>
@@ -9007,10 +8846,10 @@
         <v>187</v>
       </c>
       <c r="D80" t="s">
-        <v>10</v>
-      </c>
-      <c r="E80" t="s">
         <v>1974</v>
+      </c>
+      <c r="E80" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.3">
@@ -9024,9 +8863,6 @@
         <v>183</v>
       </c>
       <c r="D81" t="s">
-        <v>10</v>
-      </c>
-      <c r="E81" t="s">
         <v>1976</v>
       </c>
     </row>
@@ -9041,9 +8877,6 @@
         <v>185</v>
       </c>
       <c r="D82" t="s">
-        <v>10</v>
-      </c>
-      <c r="E82" t="s">
         <v>1978</v>
       </c>
     </row>
@@ -9058,9 +8891,6 @@
         <v>190</v>
       </c>
       <c r="D83" t="s">
-        <v>10</v>
-      </c>
-      <c r="E83" t="s">
         <v>1980</v>
       </c>
     </row>
@@ -9075,9 +8905,6 @@
         <v>1982</v>
       </c>
       <c r="D84" t="s">
-        <v>10</v>
-      </c>
-      <c r="E84" t="s">
         <v>1983</v>
       </c>
     </row>
@@ -9092,9 +8919,6 @@
         <v>188</v>
       </c>
       <c r="D85" t="s">
-        <v>10</v>
-      </c>
-      <c r="E85" t="s">
         <v>1985</v>
       </c>
     </row>
@@ -9109,10 +8933,10 @@
         <v>9</v>
       </c>
       <c r="D86" t="s">
-        <v>28</v>
-      </c>
-      <c r="E86" t="s">
         <v>10</v>
+      </c>
+      <c r="E86" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.3">
@@ -9126,9 +8950,6 @@
         <v>197</v>
       </c>
       <c r="D87" t="s">
-        <v>28</v>
-      </c>
-      <c r="E87" t="s">
         <v>1987</v>
       </c>
     </row>
@@ -9143,9 +8964,6 @@
         <v>200</v>
       </c>
       <c r="D88" t="s">
-        <v>28</v>
-      </c>
-      <c r="E88" t="s">
         <v>1989</v>
       </c>
     </row>
@@ -9160,9 +8978,6 @@
         <v>202</v>
       </c>
       <c r="D89" t="s">
-        <v>28</v>
-      </c>
-      <c r="E89" t="s">
         <v>1991</v>
       </c>
     </row>
@@ -9177,9 +8992,6 @@
         <v>203</v>
       </c>
       <c r="D90" t="s">
-        <v>28</v>
-      </c>
-      <c r="E90" t="s">
         <v>1993</v>
       </c>
     </row>
@@ -9194,9 +9006,6 @@
         <v>195</v>
       </c>
       <c r="D91" t="s">
-        <v>28</v>
-      </c>
-      <c r="E91" t="s">
         <v>1995</v>
       </c>
     </row>
@@ -9211,9 +9020,6 @@
         <v>192</v>
       </c>
       <c r="D92" t="s">
-        <v>28</v>
-      </c>
-      <c r="E92" t="s">
         <v>193</v>
       </c>
     </row>
@@ -9230,8 +9036,8 @@
       <c r="D93" t="s">
         <v>1847</v>
       </c>
-      <c r="E93" t="s">
-        <v>1847</v>
+      <c r="E93" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.3">
@@ -9245,9 +9051,6 @@
         <v>209</v>
       </c>
       <c r="D94" t="s">
-        <v>1847</v>
-      </c>
-      <c r="E94" t="s">
         <v>1998</v>
       </c>
     </row>
@@ -9262,9 +9065,6 @@
         <v>206</v>
       </c>
       <c r="D95" t="s">
-        <v>1847</v>
-      </c>
-      <c r="E95" t="s">
         <v>2000</v>
       </c>
     </row>
@@ -9279,9 +9079,6 @@
         <v>208</v>
       </c>
       <c r="D96" t="s">
-        <v>1847</v>
-      </c>
-      <c r="E96" t="s">
         <v>2002</v>
       </c>
     </row>
@@ -9296,9 +9093,6 @@
         <v>210</v>
       </c>
       <c r="D97" t="s">
-        <v>1847</v>
-      </c>
-      <c r="E97" t="s">
         <v>2004</v>
       </c>
     </row>
@@ -9313,9 +9107,6 @@
         <v>207</v>
       </c>
       <c r="D98" t="s">
-        <v>1847</v>
-      </c>
-      <c r="E98" t="s">
         <v>2006</v>
       </c>
     </row>
@@ -9330,10 +9121,10 @@
         <v>247</v>
       </c>
       <c r="D99" t="s">
-        <v>15</v>
-      </c>
-      <c r="E99" t="s">
         <v>248</v>
+      </c>
+      <c r="E99" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.3">
@@ -9347,9 +9138,6 @@
         <v>235</v>
       </c>
       <c r="D100" t="s">
-        <v>15</v>
-      </c>
-      <c r="E100" t="s">
         <v>236</v>
       </c>
     </row>
@@ -9364,9 +9152,6 @@
         <v>214</v>
       </c>
       <c r="D101" t="s">
-        <v>15</v>
-      </c>
-      <c r="E101" t="s">
         <v>214</v>
       </c>
     </row>
@@ -9381,9 +9166,6 @@
         <v>225</v>
       </c>
       <c r="D102" t="s">
-        <v>15</v>
-      </c>
-      <c r="E102" t="s">
         <v>2009</v>
       </c>
     </row>
@@ -9398,9 +9180,6 @@
         <v>216</v>
       </c>
       <c r="D103" t="s">
-        <v>15</v>
-      </c>
-      <c r="E103" t="s">
         <v>217</v>
       </c>
     </row>
@@ -9415,9 +9194,6 @@
         <v>229</v>
       </c>
       <c r="D104" t="s">
-        <v>15</v>
-      </c>
-      <c r="E104" t="s">
         <v>2012</v>
       </c>
     </row>
@@ -9432,9 +9208,6 @@
         <v>222</v>
       </c>
       <c r="D105" t="s">
-        <v>15</v>
-      </c>
-      <c r="E105" t="s">
         <v>223</v>
       </c>
     </row>
@@ -9449,9 +9222,6 @@
         <v>227</v>
       </c>
       <c r="D106" t="s">
-        <v>15</v>
-      </c>
-      <c r="E106" t="s">
         <v>2015</v>
       </c>
     </row>
@@ -9466,9 +9236,6 @@
         <v>2017</v>
       </c>
       <c r="D107" t="s">
-        <v>15</v>
-      </c>
-      <c r="E107" t="s">
         <v>2018</v>
       </c>
     </row>
@@ -9483,9 +9250,6 @@
         <v>249</v>
       </c>
       <c r="D108" t="s">
-        <v>15</v>
-      </c>
-      <c r="E108" t="s">
         <v>2019</v>
       </c>
     </row>
@@ -9500,9 +9264,6 @@
         <v>262</v>
       </c>
       <c r="D109" t="s">
-        <v>15</v>
-      </c>
-      <c r="E109" t="s">
         <v>2020</v>
       </c>
     </row>
@@ -9517,9 +9278,6 @@
         <v>233</v>
       </c>
       <c r="D110" t="s">
-        <v>15</v>
-      </c>
-      <c r="E110" t="s">
         <v>2022</v>
       </c>
     </row>
@@ -9534,9 +9292,6 @@
         <v>257</v>
       </c>
       <c r="D111" t="s">
-        <v>15</v>
-      </c>
-      <c r="E111" t="s">
         <v>258</v>
       </c>
     </row>
@@ -9551,9 +9306,6 @@
         <v>219</v>
       </c>
       <c r="D112" t="s">
-        <v>15</v>
-      </c>
-      <c r="E112" t="s">
         <v>220</v>
       </c>
     </row>
@@ -9568,9 +9320,6 @@
         <v>245</v>
       </c>
       <c r="D113" t="s">
-        <v>15</v>
-      </c>
-      <c r="E113" t="s">
         <v>258</v>
       </c>
     </row>
@@ -9585,9 +9334,6 @@
         <v>228</v>
       </c>
       <c r="D114" t="s">
-        <v>15</v>
-      </c>
-      <c r="E114" t="s">
         <v>103</v>
       </c>
     </row>
@@ -9602,9 +9348,6 @@
         <v>241</v>
       </c>
       <c r="D115" t="s">
-        <v>15</v>
-      </c>
-      <c r="E115" t="s">
         <v>2027</v>
       </c>
     </row>
@@ -9619,9 +9362,6 @@
         <v>238</v>
       </c>
       <c r="D116" t="s">
-        <v>15</v>
-      </c>
-      <c r="E116" t="s">
         <v>239</v>
       </c>
     </row>
@@ -9636,9 +9376,6 @@
         <v>231</v>
       </c>
       <c r="D117" t="s">
-        <v>15</v>
-      </c>
-      <c r="E117" t="s">
         <v>2030</v>
       </c>
     </row>
@@ -9653,9 +9390,6 @@
         <v>252</v>
       </c>
       <c r="D118" t="s">
-        <v>15</v>
-      </c>
-      <c r="E118" t="s">
         <v>2031</v>
       </c>
     </row>
@@ -9670,9 +9404,6 @@
         <v>212</v>
       </c>
       <c r="D119" t="s">
-        <v>15</v>
-      </c>
-      <c r="E119" t="s">
         <v>2033</v>
       </c>
     </row>
@@ -9687,9 +9418,6 @@
         <v>250</v>
       </c>
       <c r="D120" t="s">
-        <v>15</v>
-      </c>
-      <c r="E120" t="s">
         <v>2035</v>
       </c>
     </row>
@@ -9704,9 +9432,6 @@
         <v>263</v>
       </c>
       <c r="D121" t="s">
-        <v>15</v>
-      </c>
-      <c r="E121" t="s">
         <v>2037</v>
       </c>
     </row>
@@ -9721,9 +9446,6 @@
         <v>243</v>
       </c>
       <c r="D122" t="s">
-        <v>15</v>
-      </c>
-      <c r="E122" t="s">
         <v>2038</v>
       </c>
     </row>
@@ -9738,9 +9460,6 @@
         <v>254</v>
       </c>
       <c r="D123" t="s">
-        <v>15</v>
-      </c>
-      <c r="E123" t="s">
         <v>255</v>
       </c>
     </row>
@@ -9755,9 +9474,6 @@
         <v>265</v>
       </c>
       <c r="D124" t="s">
-        <v>15</v>
-      </c>
-      <c r="E124" t="s">
         <v>266</v>
       </c>
     </row>
@@ -9772,9 +9488,6 @@
         <v>260</v>
       </c>
       <c r="D125" t="s">
-        <v>15</v>
-      </c>
-      <c r="E125" t="s">
         <v>2042</v>
       </c>
     </row>
@@ -9789,10 +9502,10 @@
         <v>275</v>
       </c>
       <c r="D126" t="s">
-        <v>31</v>
-      </c>
-      <c r="E126" t="s">
         <v>2043</v>
+      </c>
+      <c r="E126" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.3">
@@ -9806,9 +9519,6 @@
         <v>276</v>
       </c>
       <c r="D127" t="s">
-        <v>31</v>
-      </c>
-      <c r="E127" t="s">
         <v>2045</v>
       </c>
     </row>
@@ -9823,13 +9533,10 @@
         <v>268</v>
       </c>
       <c r="D128" t="s">
-        <v>31</v>
-      </c>
-      <c r="E128" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>1858</v>
       </c>
@@ -9840,13 +9547,10 @@
         <v>270</v>
       </c>
       <c r="D129" t="s">
-        <v>31</v>
-      </c>
-      <c r="E129" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>1858</v>
       </c>
@@ -9857,16 +9561,13 @@
         <v>273</v>
       </c>
       <c r="D130" t="s">
-        <v>31</v>
-      </c>
-      <c r="E130" t="s">
         <v>2047</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="B1 C1:D1" numberStoredAsText="1"/>
+    <ignoredError sqref="B1 C1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -9875,8 +9576,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:C749"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -18137,8 +17838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E389"/>
   <sheetViews>
-    <sheetView topLeftCell="A424" workbookViewId="0">
-      <selection sqref="A1:E389"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A72" sqref="A72:E72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -24765,4 +24466,220 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79703D5B-C890-40E5-A228-DD50F9AC0CE1}">
+  <dimension ref="A1:C18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="10.8984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>1695</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2256</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1725</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>2075</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>1713</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>1751</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>2117</v>
+      </c>
+      <c r="B6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>2257</v>
+      </c>
+      <c r="B7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>1769</v>
+      </c>
+      <c r="B8" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>2157</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>2148</v>
+      </c>
+      <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>1770</v>
+      </c>
+      <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>2158</v>
+      </c>
+      <c r="B12" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>1773</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>2259</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>2260</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+      <c r="C15">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>2261</v>
+      </c>
+      <c r="B16" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>2258</v>
+      </c>
+      <c r="B17" t="s">
+        <v>14</v>
+      </c>
+      <c r="C17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>2262</v>
+      </c>
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>